<commit_message>
Retraining the model for Horeco
</commit_message>
<xml_diff>
--- a/Horeco/Results_Production_Horeco_xgb.xlsx
+++ b/Horeco/Results_Production_Horeco_xgb.xlsx
@@ -28,162 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>24.01.20269</t>
-  </si>
-  <si>
-    <t>24.01.202610</t>
-  </si>
-  <si>
-    <t>24.01.202611</t>
-  </si>
-  <si>
-    <t>24.01.202612</t>
-  </si>
-  <si>
-    <t>24.01.202613</t>
-  </si>
-  <si>
-    <t>24.01.202614</t>
-  </si>
-  <si>
-    <t>24.01.202615</t>
-  </si>
-  <si>
-    <t>24.01.202616</t>
-  </si>
-  <si>
-    <t>24.01.202617</t>
-  </si>
-  <si>
-    <t>24.01.202618</t>
-  </si>
-  <si>
-    <t>24.01.202619</t>
-  </si>
-  <si>
-    <t>24.01.202620</t>
-  </si>
-  <si>
-    <t>24.01.202621</t>
-  </si>
-  <si>
-    <t>24.01.202622</t>
-  </si>
-  <si>
-    <t>24.01.202623</t>
-  </si>
-  <si>
-    <t>24.01.202624</t>
-  </si>
-  <si>
-    <t>25.01.20261</t>
-  </si>
-  <si>
-    <t>25.01.20262</t>
-  </si>
-  <si>
-    <t>25.01.20263</t>
-  </si>
-  <si>
-    <t>25.01.20264</t>
-  </si>
-  <si>
-    <t>25.01.20265</t>
-  </si>
-  <si>
-    <t>25.01.20266</t>
-  </si>
-  <si>
-    <t>25.01.20267</t>
-  </si>
-  <si>
-    <t>25.01.20268</t>
-  </si>
-  <si>
-    <t>25.01.20269</t>
-  </si>
-  <si>
-    <t>25.01.202610</t>
-  </si>
-  <si>
-    <t>25.01.202611</t>
-  </si>
-  <si>
-    <t>25.01.202612</t>
-  </si>
-  <si>
-    <t>25.01.202613</t>
-  </si>
-  <si>
-    <t>25.01.202614</t>
-  </si>
-  <si>
-    <t>25.01.202615</t>
-  </si>
-  <si>
-    <t>25.01.202616</t>
-  </si>
-  <si>
-    <t>25.01.202617</t>
-  </si>
-  <si>
-    <t>25.01.202618</t>
-  </si>
-  <si>
-    <t>25.01.202619</t>
-  </si>
-  <si>
-    <t>25.01.202620</t>
-  </si>
-  <si>
-    <t>25.01.202621</t>
-  </si>
-  <si>
-    <t>25.01.202622</t>
-  </si>
-  <si>
-    <t>25.01.202623</t>
-  </si>
-  <si>
-    <t>25.01.202624</t>
-  </si>
-  <si>
-    <t>26.01.20261</t>
-  </si>
-  <si>
-    <t>26.01.20262</t>
-  </si>
-  <si>
-    <t>26.01.20263</t>
-  </si>
-  <si>
-    <t>26.01.20264</t>
-  </si>
-  <si>
-    <t>26.01.20265</t>
-  </si>
-  <si>
-    <t>26.01.20266</t>
-  </si>
-  <si>
-    <t>26.01.20267</t>
-  </si>
-  <si>
-    <t>26.01.20268</t>
-  </si>
-  <si>
-    <t>26.01.20269</t>
-  </si>
-  <si>
-    <t>26.01.202610</t>
-  </si>
-  <si>
-    <t>26.01.202611</t>
-  </si>
-  <si>
-    <t>26.01.202612</t>
-  </si>
-  <si>
     <t>26.01.202613</t>
   </si>
   <si>
@@ -533,6 +377,162 @@
   </si>
   <si>
     <t>31.01.20269</t>
+  </si>
+  <si>
+    <t>31.01.202610</t>
+  </si>
+  <si>
+    <t>31.01.202611</t>
+  </si>
+  <si>
+    <t>31.01.202612</t>
+  </si>
+  <si>
+    <t>31.01.202613</t>
+  </si>
+  <si>
+    <t>31.01.202614</t>
+  </si>
+  <si>
+    <t>31.01.202615</t>
+  </si>
+  <si>
+    <t>31.01.202616</t>
+  </si>
+  <si>
+    <t>31.01.202617</t>
+  </si>
+  <si>
+    <t>31.01.202618</t>
+  </si>
+  <si>
+    <t>31.01.202619</t>
+  </si>
+  <si>
+    <t>31.01.202620</t>
+  </si>
+  <si>
+    <t>31.01.202621</t>
+  </si>
+  <si>
+    <t>31.01.202622</t>
+  </si>
+  <si>
+    <t>31.01.202623</t>
+  </si>
+  <si>
+    <t>31.01.202624</t>
+  </si>
+  <si>
+    <t>01.02.20261</t>
+  </si>
+  <si>
+    <t>01.02.20262</t>
+  </si>
+  <si>
+    <t>01.02.20263</t>
+  </si>
+  <si>
+    <t>01.02.20264</t>
+  </si>
+  <si>
+    <t>01.02.20265</t>
+  </si>
+  <si>
+    <t>01.02.20266</t>
+  </si>
+  <si>
+    <t>01.02.20267</t>
+  </si>
+  <si>
+    <t>01.02.20268</t>
+  </si>
+  <si>
+    <t>01.02.20269</t>
+  </si>
+  <si>
+    <t>01.02.202610</t>
+  </si>
+  <si>
+    <t>01.02.202611</t>
+  </si>
+  <si>
+    <t>01.02.202612</t>
+  </si>
+  <si>
+    <t>01.02.202613</t>
+  </si>
+  <si>
+    <t>01.02.202614</t>
+  </si>
+  <si>
+    <t>01.02.202615</t>
+  </si>
+  <si>
+    <t>01.02.202616</t>
+  </si>
+  <si>
+    <t>01.02.202617</t>
+  </si>
+  <si>
+    <t>01.02.202618</t>
+  </si>
+  <si>
+    <t>01.02.202619</t>
+  </si>
+  <si>
+    <t>01.02.202620</t>
+  </si>
+  <si>
+    <t>01.02.202621</t>
+  </si>
+  <si>
+    <t>01.02.202622</t>
+  </si>
+  <si>
+    <t>01.02.202623</t>
+  </si>
+  <si>
+    <t>01.02.202624</t>
+  </si>
+  <si>
+    <t>02.02.20261</t>
+  </si>
+  <si>
+    <t>02.02.20262</t>
+  </si>
+  <si>
+    <t>02.02.20263</t>
+  </si>
+  <si>
+    <t>02.02.20264</t>
+  </si>
+  <si>
+    <t>02.02.20265</t>
+  </si>
+  <si>
+    <t>02.02.20266</t>
+  </si>
+  <si>
+    <t>02.02.20267</t>
+  </si>
+  <si>
+    <t>02.02.20268</t>
+  </si>
+  <si>
+    <t>02.02.20269</t>
+  </si>
+  <si>
+    <t>02.02.202610</t>
+  </si>
+  <si>
+    <t>02.02.202611</t>
+  </si>
+  <si>
+    <t>02.02.202612</t>
+  </si>
+  <si>
+    <t>02.02.202613</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>0.174</v>
+        <v>0.11</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>0.187</v>
+        <v>0.098</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>0.2</v>
+        <v>0.058</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>0.219</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>0.074</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>0.021</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,10 +1056,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>46046</v>
+        <v>46048</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>46046</v>
+        <v>46049</v>
       </c>
       <c r="B14">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>46046</v>
+        <v>46049</v>
       </c>
       <c r="B15">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>46046</v>
+        <v>46049</v>
       </c>
       <c r="B16">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>46046</v>
+        <v>46049</v>
       </c>
       <c r="B17">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1182,10 +1182,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1196,10 +1196,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1210,10 +1210,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>0.058</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>0.079</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>0.128</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>0.083</v>
+        <v>0.142</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>0.251</v>
+        <v>0.136</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B29">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>0.473</v>
+        <v>0.093</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B30">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>0.517</v>
+        <v>0.058</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B31">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>0.659</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B32">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>0.608</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B33">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C33">
-        <v>0.516</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B34">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>0.256</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C35">
-        <v>0.058</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B36">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>46047</v>
+        <v>46049</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>46047</v>
+        <v>46050</v>
       </c>
       <c r="B38">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>46047</v>
+        <v>46050</v>
       </c>
       <c r="B39">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>46047</v>
+        <v>46050</v>
       </c>
       <c r="B40">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>46047</v>
+        <v>46050</v>
       </c>
       <c r="B41">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1518,10 +1518,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B45">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>0.093</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>0.272</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>0.589</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B50">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>0.758</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B51">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C51">
-        <v>0.042</v>
+        <v>0.88</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C52">
-        <v>0.098</v>
+        <v>0.835</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B53">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>0.136</v>
+        <v>0.556</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B54">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>0.174</v>
+        <v>0.306</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B55">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C55">
-        <v>0.178</v>
+        <v>0.064</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B56">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>0.174</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B57">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>0.098</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B58">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>0.058</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B59">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B60">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B61">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>46048</v>
+        <v>46051</v>
       </c>
       <c r="B62">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>46048</v>
+        <v>46051</v>
       </c>
       <c r="B63">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>46048</v>
+        <v>46051</v>
       </c>
       <c r="B64">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>46048</v>
+        <v>46051</v>
       </c>
       <c r="B65">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,10 +1840,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1854,10 +1854,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1868,10 +1868,10 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B70">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B71">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>0.116</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B72">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>0.433</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>0.755</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B74">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1.124</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B75">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C75">
-        <v>0.042</v>
+        <v>1.127</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B76">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C76">
-        <v>0.102</v>
+        <v>1.04</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B77">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C77">
-        <v>0.178</v>
+        <v>0.714</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B78">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C78">
-        <v>0.198</v>
+        <v>0.38</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B79">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C79">
-        <v>0.185</v>
+        <v>0.074</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B80">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C80">
-        <v>0.174</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B81">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C81">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B82">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C82">
-        <v>0.058</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B83">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2064,10 +2064,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B84">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B85">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>46049</v>
+        <v>46052</v>
       </c>
       <c r="B86">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>46049</v>
+        <v>46052</v>
       </c>
       <c r="B87">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>46049</v>
+        <v>46052</v>
       </c>
       <c r="B88">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>46049</v>
+        <v>46052</v>
       </c>
       <c r="B89">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B92">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2190,10 +2190,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2204,10 +2204,10 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B94">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B95">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B96">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B97">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>0.167</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B98">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>0.193</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B99">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C99">
-        <v>0.093</v>
+        <v>0.2</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B100">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C100">
-        <v>0.264</v>
+        <v>0.188</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B101">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C101">
-        <v>0.541</v>
+        <v>0.116</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B102">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C102">
-        <v>0.783</v>
+        <v>0.064</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B103">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C103">
-        <v>1.049</v>
+        <v>0.012</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B104">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C104">
-        <v>1.049</v>
+        <v>0</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B105">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C105">
-        <v>0.648</v>
+        <v>0</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B106">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>0.448</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B107">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>0.089</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B108">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B109">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>46050</v>
+        <v>46053</v>
       </c>
       <c r="B110">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>46050</v>
+        <v>46053</v>
       </c>
       <c r="B111">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>46050</v>
+        <v>46053</v>
       </c>
       <c r="B112">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>46050</v>
+        <v>46053</v>
       </c>
       <c r="B113">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B115">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2512,10 +2512,10 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -2526,10 +2526,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B117">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B118">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B119">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B120">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>0.253</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B121">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>0.404</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B122">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B123">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C123">
-        <v>0.058</v>
+        <v>0.543</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B124">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C124">
-        <v>0.227</v>
+        <v>0.555</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B125">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C125">
-        <v>0.432</v>
+        <v>0.514</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B126">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C126">
-        <v>0.58</v>
+        <v>0.307</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B127">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C127">
-        <v>1.049</v>
+        <v>0.074</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B128">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C128">
-        <v>1.049</v>
+        <v>0</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B129">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C129">
-        <v>0.768</v>
+        <v>0</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B130">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C130">
-        <v>0.397</v>
+        <v>0</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B131">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C131">
-        <v>0.089</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B132">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>46051</v>
+        <v>46053</v>
       </c>
       <c r="B133">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>46051</v>
+        <v>46054</v>
       </c>
       <c r="B134">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>46051</v>
+        <v>46054</v>
       </c>
       <c r="B135">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>46051</v>
+        <v>46054</v>
       </c>
       <c r="B136">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>46051</v>
+        <v>46054</v>
       </c>
       <c r="B137">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B139">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2848,10 +2848,10 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B140">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -2862,10 +2862,10 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B141">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -2876,10 +2876,10 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B142">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B143">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>0.094</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B144">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>0.281</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B145">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B146">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>0.548</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B147">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C147">
-        <v>0.064</v>
+        <v>0.506</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B148">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C148">
-        <v>0.201</v>
+        <v>0.483</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B149">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C149">
-        <v>0.437</v>
+        <v>0.382</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B150">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C150">
-        <v>0.536</v>
+        <v>0.244</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B151">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C151">
-        <v>0.536</v>
+        <v>0.058</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B152">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C152">
-        <v>0.437</v>
+        <v>0</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B153">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C153">
-        <v>0.208</v>
+        <v>0</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B154">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C154">
-        <v>0.116</v>
+        <v>0</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B155">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C155">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B156">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="B157">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="B158">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="B159">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="B160">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="B161">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B163">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3184,10 +3184,10 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B164">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -3198,10 +3198,10 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B165">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -3212,10 +3212,10 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B166">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B167">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>0.058</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B168">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>0.198</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B169">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="B170">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C170">
-        <v>0</v>
+        <v>0.402</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Updating the model for Horeco
</commit_message>
<xml_diff>
--- a/Horeco/Results_Production_Horeco_xgb.xlsx
+++ b/Horeco/Results_Production_Horeco_xgb.xlsx
@@ -28,201 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>18.02.202617</t>
-  </si>
-  <si>
-    <t>18.02.202618</t>
-  </si>
-  <si>
-    <t>18.02.202619</t>
-  </si>
-  <si>
-    <t>18.02.202620</t>
-  </si>
-  <si>
-    <t>18.02.202621</t>
-  </si>
-  <si>
-    <t>18.02.202622</t>
-  </si>
-  <si>
-    <t>18.02.202623</t>
-  </si>
-  <si>
-    <t>18.02.202624</t>
-  </si>
-  <si>
-    <t>19.02.20261</t>
-  </si>
-  <si>
-    <t>19.02.20262</t>
-  </si>
-  <si>
-    <t>19.02.20263</t>
-  </si>
-  <si>
-    <t>19.02.20264</t>
-  </si>
-  <si>
-    <t>19.02.20265</t>
-  </si>
-  <si>
-    <t>19.02.20266</t>
-  </si>
-  <si>
-    <t>19.02.20267</t>
-  </si>
-  <si>
-    <t>19.02.20268</t>
-  </si>
-  <si>
-    <t>19.02.20269</t>
-  </si>
-  <si>
-    <t>19.02.202610</t>
-  </si>
-  <si>
-    <t>19.02.202611</t>
-  </si>
-  <si>
-    <t>19.02.202612</t>
-  </si>
-  <si>
-    <t>19.02.202613</t>
-  </si>
-  <si>
-    <t>19.02.202614</t>
-  </si>
-  <si>
-    <t>19.02.202615</t>
-  </si>
-  <si>
-    <t>19.02.202616</t>
-  </si>
-  <si>
-    <t>19.02.202617</t>
-  </si>
-  <si>
-    <t>19.02.202618</t>
-  </si>
-  <si>
-    <t>19.02.202619</t>
-  </si>
-  <si>
-    <t>19.02.202620</t>
-  </si>
-  <si>
-    <t>19.02.202621</t>
-  </si>
-  <si>
-    <t>19.02.202622</t>
-  </si>
-  <si>
-    <t>19.02.202623</t>
-  </si>
-  <si>
-    <t>19.02.202624</t>
-  </si>
-  <si>
-    <t>20.02.20261</t>
-  </si>
-  <si>
-    <t>20.02.20262</t>
-  </si>
-  <si>
-    <t>20.02.20263</t>
-  </si>
-  <si>
-    <t>20.02.20264</t>
-  </si>
-  <si>
-    <t>20.02.20265</t>
-  </si>
-  <si>
-    <t>20.02.20266</t>
-  </si>
-  <si>
-    <t>20.02.20267</t>
-  </si>
-  <si>
-    <t>20.02.20268</t>
-  </si>
-  <si>
-    <t>20.02.20269</t>
-  </si>
-  <si>
-    <t>20.02.202610</t>
-  </si>
-  <si>
-    <t>20.02.202611</t>
-  </si>
-  <si>
-    <t>20.02.202612</t>
-  </si>
-  <si>
-    <t>20.02.202613</t>
-  </si>
-  <si>
-    <t>20.02.202614</t>
-  </si>
-  <si>
-    <t>20.02.202615</t>
-  </si>
-  <si>
-    <t>20.02.202616</t>
-  </si>
-  <si>
-    <t>20.02.202617</t>
-  </si>
-  <si>
-    <t>20.02.202618</t>
-  </si>
-  <si>
-    <t>20.02.202619</t>
-  </si>
-  <si>
-    <t>20.02.202620</t>
-  </si>
-  <si>
-    <t>20.02.202621</t>
-  </si>
-  <si>
-    <t>20.02.202622</t>
-  </si>
-  <si>
-    <t>20.02.202623</t>
-  </si>
-  <si>
-    <t>20.02.202624</t>
-  </si>
-  <si>
-    <t>21.02.20261</t>
-  </si>
-  <si>
-    <t>21.02.20262</t>
-  </si>
-  <si>
-    <t>21.02.20263</t>
-  </si>
-  <si>
-    <t>21.02.20264</t>
-  </si>
-  <si>
-    <t>21.02.20265</t>
-  </si>
-  <si>
-    <t>21.02.20266</t>
-  </si>
-  <si>
-    <t>21.02.20267</t>
-  </si>
-  <si>
-    <t>21.02.20268</t>
-  </si>
-  <si>
-    <t>21.02.20269</t>
-  </si>
-  <si>
     <t>21.02.202610</t>
   </si>
   <si>
@@ -533,6 +338,201 @@
   </si>
   <si>
     <t>25.02.202617</t>
+  </si>
+  <si>
+    <t>25.02.202618</t>
+  </si>
+  <si>
+    <t>25.02.202619</t>
+  </si>
+  <si>
+    <t>25.02.202620</t>
+  </si>
+  <si>
+    <t>25.02.202621</t>
+  </si>
+  <si>
+    <t>25.02.202622</t>
+  </si>
+  <si>
+    <t>25.02.202623</t>
+  </si>
+  <si>
+    <t>25.02.202624</t>
+  </si>
+  <si>
+    <t>26.02.20261</t>
+  </si>
+  <si>
+    <t>26.02.20262</t>
+  </si>
+  <si>
+    <t>26.02.20263</t>
+  </si>
+  <si>
+    <t>26.02.20264</t>
+  </si>
+  <si>
+    <t>26.02.20265</t>
+  </si>
+  <si>
+    <t>26.02.20266</t>
+  </si>
+  <si>
+    <t>26.02.20267</t>
+  </si>
+  <si>
+    <t>26.02.20268</t>
+  </si>
+  <si>
+    <t>26.02.20269</t>
+  </si>
+  <si>
+    <t>26.02.202610</t>
+  </si>
+  <si>
+    <t>26.02.202611</t>
+  </si>
+  <si>
+    <t>26.02.202612</t>
+  </si>
+  <si>
+    <t>26.02.202613</t>
+  </si>
+  <si>
+    <t>26.02.202614</t>
+  </si>
+  <si>
+    <t>26.02.202615</t>
+  </si>
+  <si>
+    <t>26.02.202616</t>
+  </si>
+  <si>
+    <t>26.02.202617</t>
+  </si>
+  <si>
+    <t>26.02.202618</t>
+  </si>
+  <si>
+    <t>26.02.202619</t>
+  </si>
+  <si>
+    <t>26.02.202620</t>
+  </si>
+  <si>
+    <t>26.02.202621</t>
+  </si>
+  <si>
+    <t>26.02.202622</t>
+  </si>
+  <si>
+    <t>26.02.202623</t>
+  </si>
+  <si>
+    <t>26.02.202624</t>
+  </si>
+  <si>
+    <t>27.02.20261</t>
+  </si>
+  <si>
+    <t>27.02.20262</t>
+  </si>
+  <si>
+    <t>27.02.20263</t>
+  </si>
+  <si>
+    <t>27.02.20264</t>
+  </si>
+  <si>
+    <t>27.02.20265</t>
+  </si>
+  <si>
+    <t>27.02.20266</t>
+  </si>
+  <si>
+    <t>27.02.20267</t>
+  </si>
+  <si>
+    <t>27.02.20268</t>
+  </si>
+  <si>
+    <t>27.02.20269</t>
+  </si>
+  <si>
+    <t>27.02.202610</t>
+  </si>
+  <si>
+    <t>27.02.202611</t>
+  </si>
+  <si>
+    <t>27.02.202612</t>
+  </si>
+  <si>
+    <t>27.02.202613</t>
+  </si>
+  <si>
+    <t>27.02.202614</t>
+  </si>
+  <si>
+    <t>27.02.202615</t>
+  </si>
+  <si>
+    <t>27.02.202616</t>
+  </si>
+  <si>
+    <t>27.02.202617</t>
+  </si>
+  <si>
+    <t>27.02.202618</t>
+  </si>
+  <si>
+    <t>27.02.202619</t>
+  </si>
+  <si>
+    <t>27.02.202620</t>
+  </si>
+  <si>
+    <t>27.02.202621</t>
+  </si>
+  <si>
+    <t>27.02.202622</t>
+  </si>
+  <si>
+    <t>27.02.202623</t>
+  </si>
+  <si>
+    <t>27.02.202624</t>
+  </si>
+  <si>
+    <t>28.02.20261</t>
+  </si>
+  <si>
+    <t>28.02.20262</t>
+  </si>
+  <si>
+    <t>28.02.20263</t>
+  </si>
+  <si>
+    <t>28.02.20264</t>
+  </si>
+  <si>
+    <t>28.02.20265</t>
+  </si>
+  <si>
+    <t>28.02.20266</t>
+  </si>
+  <si>
+    <t>28.02.20267</t>
+  </si>
+  <si>
+    <t>28.02.20268</t>
+  </si>
+  <si>
+    <t>28.02.20269</t>
+  </si>
+  <si>
+    <t>28.02.202610</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.058</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.174</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.232</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.232</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B8">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.218</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>46071</v>
+        <v>46074</v>
       </c>
       <c r="B9">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.178</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.083</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1056,10 +1056,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>46072</v>
+        <v>46074</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>0.368</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>0.925</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>1.348</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B22">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>1.366</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B23">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>1.353</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>1.304</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B25">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>1.007</v>
+        <v>0.034</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B26">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>0.449</v>
+        <v>0.185</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>0.174</v>
+        <v>0.347</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B28">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>0.021</v>
+        <v>0.655</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B29">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1.234</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B30">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1.304</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B31">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1.299</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B32">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1.132</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>46072</v>
+        <v>46075</v>
       </c>
       <c r="B33">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.495</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>46073</v>
+        <v>46075</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.231</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>46073</v>
+        <v>46075</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>46073</v>
+        <v>46075</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>46073</v>
+        <v>46075</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>46073</v>
+        <v>46075</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>46073</v>
+        <v>46075</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>46073</v>
+        <v>46075</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>0.042</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B43">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>0.527</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B45">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>1.007</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B46">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>1.151</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B47">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B48">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>1.127</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B49">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>0.489</v>
+        <v>0.061</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B50">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>0.274</v>
+        <v>0.24</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>0.099</v>
+        <v>0.444</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B52">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>0.502</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B53">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>0.493</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B54">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>0.493</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B55">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>0.475</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B56">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>0.402</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="B57">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>0.238</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>46074</v>
+        <v>46076</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>0.098</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>46074</v>
+        <v>46076</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>46074</v>
+        <v>46076</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>46074</v>
+        <v>46076</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>46074</v>
+        <v>46076</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>46074</v>
+        <v>46076</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>46074</v>
+        <v>46076</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>0.194</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>0.321</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B69">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>0.614</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B70">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>1.04</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B71">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>1.047</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B72">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>1.034</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B73">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>0.481</v>
+        <v>0.042</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B74">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>0.285</v>
+        <v>0.185</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B75">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>0.142</v>
+        <v>0.402</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B76">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>0.015</v>
+        <v>0.598</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B77">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1.004</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B78">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>0.794</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B79">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>0.497</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B80">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>0.441</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>46074</v>
+        <v>46077</v>
       </c>
       <c r="B81">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>46075</v>
+        <v>46077</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>0.102</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>46075</v>
+        <v>46077</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2064,10 +2064,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>46075</v>
+        <v>46077</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>46075</v>
+        <v>46077</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>46075</v>
+        <v>46077</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>46075</v>
+        <v>46077</v>
       </c>
       <c r="B87">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>46075</v>
+        <v>46077</v>
       </c>
       <c r="B88">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B89">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B90">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B91">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>0.185</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B92">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>0.453</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B93">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C93">
-        <v>0.97</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B94">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>1.142</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B95">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C95">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B96">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>1.189</v>
+        <v>0</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B97">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>1.034</v>
+        <v>0.044</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B98">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C98">
-        <v>0.509</v>
+        <v>0.25</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B99">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C99">
-        <v>0.211</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B100">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C100">
-        <v>0.025</v>
+        <v>1.029</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B101">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>1.255</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B102">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>1.138</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B103">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>0.871</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B104">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>0.679</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>46075</v>
+        <v>46078</v>
       </c>
       <c r="B105">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>0.497</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>46076</v>
+        <v>46078</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>46076</v>
+        <v>46078</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.021</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>46076</v>
+        <v>46078</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>46076</v>
+        <v>46078</v>
       </c>
       <c r="B109">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>46076</v>
+        <v>46078</v>
       </c>
       <c r="B110">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>46076</v>
+        <v>46078</v>
       </c>
       <c r="B111">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>46076</v>
+        <v>46078</v>
       </c>
       <c r="B112">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B113">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B114">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C114">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B115">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>0.178</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B116">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>0.402</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B117">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>0.52</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B118">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>0.673</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B119">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>0.789</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B120">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <v>0.648</v>
+        <v>0</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B121">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C121">
-        <v>0.484</v>
+        <v>0.064</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B122">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C122">
-        <v>0.251</v>
+        <v>0.46</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B123">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C123">
-        <v>0.098</v>
+        <v>1.079</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B124">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B125">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>1.55</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B126">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>1.515</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B127">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>1.427</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B128">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>1.262</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>46076</v>
+        <v>46079</v>
       </c>
       <c r="B129">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>0.795</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>46077</v>
+        <v>46079</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>0.316</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>46077</v>
+        <v>46079</v>
       </c>
       <c r="B131">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.034</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>46077</v>
+        <v>46079</v>
       </c>
       <c r="B132">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>46077</v>
+        <v>46079</v>
       </c>
       <c r="B133">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>46077</v>
+        <v>46079</v>
       </c>
       <c r="B134">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>46077</v>
+        <v>46079</v>
       </c>
       <c r="B135">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>46077</v>
+        <v>46079</v>
       </c>
       <c r="B136">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B137">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B138">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C138">
-        <v>0.042</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B139">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>0.213</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B140">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C140">
-        <v>0.474</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B141">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C141">
-        <v>0.649</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B142">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C142">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B143">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B144">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C144">
-        <v>0.724</v>
+        <v>0</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B145">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>0.5600000000000001</v>
+        <v>0.064</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B146">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C146">
-        <v>0.369</v>
+        <v>0.483</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B147">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C147">
-        <v>0.116</v>
+        <v>1.042</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B148">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>1.313</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B149">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>1.473</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B150">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>1.499</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B151">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>1.453</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B152">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>1.33</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="B153">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>46078</v>
+        <v>46080</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>0.328</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>46078</v>
+        <v>46080</v>
       </c>
       <c r="B155">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>46078</v>
+        <v>46080</v>
       </c>
       <c r="B156">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>46078</v>
+        <v>46080</v>
       </c>
       <c r="B157">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>46078</v>
+        <v>46080</v>
       </c>
       <c r="B158">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>46078</v>
+        <v>46080</v>
       </c>
       <c r="B159">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>46078</v>
+        <v>46080</v>
       </c>
       <c r="B160">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B161">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B162">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C162">
-        <v>0.058</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B163">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C163">
-        <v>0.264</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B164">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>0.5679999999999999</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B165">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C165">
-        <v>1.116</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B166">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C166">
-        <v>1.332</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B167">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>1.332</v>
+        <v>0</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B168">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C168">
-        <v>1.318</v>
+        <v>0</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B169">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C169">
-        <v>1.093</v>
+        <v>0.094</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>46078</v>
+        <v>46081</v>
       </c>
       <c r="B170">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C170">
-        <v>0.612</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>